<commit_message>
changed model to vocab-trained one
</commit_message>
<xml_diff>
--- a/transcriptions.xlsx
+++ b/transcriptions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,312 +440,1680 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ003_dupont_01</t>
+          <t>vo_NTAQ105_2_mualani_02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Don't worry, I got this covered.</t>
+          <t>If there's one thing the Abyss fears, it's strength. If they think we're easy prey, they've got another thing coming.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_ceasth_02</t>
+          <t>vo_NTAQ104_8_nightmare_01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>No, don't look this way. I'm supposed to be hiding, remember? Captain's orders.</t>
+          <t>You come to me with many questions... and you shall be rewarded for your bravery. Ask, and you shall have the knowledge you seek.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_ceasth_01</t>
+          <t>vo_NTAQ104_7_nightmare_12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>How could they switch without me noticing...</t>
+          <t>It was an incredibly crude and painful method, but I managed to absorb some of that power. Now, I can speak to you like this and provide you with aid.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ001_istress_01</t>
+          <t>vo_NTAQ104_7_nightmare_06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I was looking to switch up my skincare routine anyway. I'm gonna try this out as soon as I get home tonight.</t>
+          <t>No... An additional soul was affected. It tried to take refuge in the missing part of your friend's soul, but was ultimately expelled</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ001_aurillac_01</t>
+          <t>vo_NTAQ105_3_nightmare_24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I'm buying for a friend, but I just wanna check... This is designed for both women and men, right?</t>
+          <t>Thank you for saying that, but there is nothing you can do.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_05</t>
+          <t>vo_NTAQ108_5_xilonen_01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Indeed. Actually, I often forget just how much older I am than you...</t>
+          <t>The Children of Echoes' territory is secure. Almosters down</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_04</t>
+          <t>vo_NTAQ105_3_nightmare_18</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ah, well, I won't lie. I've always seen myself that way.</t>
+          <t>The ruler of death cares little for the time and manner of her death. She simply guarantees that it will occur.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_06</t>
+          <t>vo_NTAQ105_3_nightmare_19</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Yes, and uh... from the surface to the ocean floor, on occasion.</t>
+          <t>Fate may be able to influence the timing... but that is all the Traveler can change.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_07</t>
+          <t>vo_NTAQ105_3_nightmare_31</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>...Apologies, that was merely an attempt at humor. You can disregard what I said.</t>
+          <t>Your thanks are unnecessary. This is the least that a magi could do.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_03</t>
+          <t>vo_NTAQ105_3_nightmare_25</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>I am most relieved to hear it.</t>
+          <t>How many years of life are enough? Ten? One hundred? One thousand? Ten thousand?</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_02</t>
+          <t>vo_NTAQ104_7_nightmare_07</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sigewinne seems to be in good spirits. I trust work hasn't been too hard on her lately?</t>
+          <t>However, this soul does not hail from that land or the Night Kingdom. Its origins remain a mystery to me.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_houilles_01</t>
+          <t>vo_NTAQ104_7_nightmare_13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Such as rebuilding the Ley Lines once more at the cost of my own existence</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ001_anais_01</t>
+          <t>vo_NTAQ105_2_mualani_03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aw, I wish I'd saved up my pocket money...</t>
+          <t>Oh! Someone's calling us...</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ004_neuvillette_01</t>
+          <t>vo_dialog_NTAQ106_wisa_01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>On behalf of the Marechaussee Phantom, I would like to once again thank the Fortress of Meropide for your assistance in the response to yesterday's prisonbreak.</t>
+          <t>No! I don't want to go! I want to stay with you!</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_bertram_01</t>
+          <t>vo_NTAQ105_2_mualani_01</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>If my research project works out, the development of underwater spaces should become much easier...</t>
+          <t>It's definitely unusual, and we should all be careful. But don't worry too much, you have us by your side.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_honore_01</t>
+          <t>vo_NTAQ104_7_nightmare_05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>And yet, his soul remains in one piece. He managed to overcome this obstacle through sheer strife of will — a truly impressive feat for a human being.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_odilon_01</t>
+          <t>vo_NTAQ104_7_nightmare_11</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>And now, the structure of the Ley Lines has also completely changed. I am the only possible vehicle for the power generated by the device.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_audree_01</t>
+          <t>vo_NTAQ108_5_xilonen_02</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Well? I've told you everything I know. Don't you think it's time for you to go looking for him? ...Not that I care, obviously.</t>
+          <t>More Abyss Tumors have descended, all near the Stadium! Let's split up and take them out!</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ001_calcagni_01</t>
+          <t>vo_NTAQ105_3_nightmare_27</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Stocks are running low, so purchase soon to avoid disappointment!</t>
+          <t>Times like these always fill me with admiration and reinforce my commitment to the mandate by shoulder</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_sigewinne_01</t>
+          <t>vo_NTAQ105_3_nightmare_26</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>I'll take care of her. Fetch me some hot water, if you would.</t>
+          <t>The Night Kingdom will disappear. The humans will continue to fight against the Abyss, and in the end, all will cease to exist. When you consider all of that, extending my life is meaningless.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ001_odilon_01</t>
+          <t>vo_NTAQ105_3_nightmare_32</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>This is the observation ward. If you want to visit a patient, you'll need authorization from the head nurse.</t>
+          <t>Time for you to leave... It's getting dark</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_morgane_01</t>
+          <t>vo_NTAQ108_5_xilonen_03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>What the heck is going on...</t>
+          <t>We need someone to guard the mean entrance</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_antibes_01</t>
+          <t>vo_NTAQ104_7_nightmare_10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Gonna have to cut this chat short — I have a patent application to write.</t>
+          <t>Back then, this method was rather ineffective. They lacked the skills to navigate the intricate structure of the Ley Lines.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ003_morgane_01</t>
+          <t>vo_NTAQ104_7_nightmare_04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Join the Head Nurse inside. If he tries anything, anything at all, shout.</t>
+          <t>Most of you are unaffected because your souls are intact. But, with a damaged soul, the effect on your friend was heightened and his soul almost shattered as a result.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ002_wriothesley_01</t>
+          <t>vo_dialog_NTAQ106_wisa_02</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Looks like our head nurse is relying on you for this one. Thanks in advance.</t>
+          <t>Hehe... No, I won't go!</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>vo_dialog_SGWLQ003_ceasth_01</t>
+          <t>vo_NTAQ104_7_nightmare_14</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>I don't trust this guy much. Be careful.</t>
+          <t>The people of Natlan worship me, and call me their lord. In the ancient past, before we died out, we were also known by a different name —angels.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_3_solnev_01</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>...</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_22</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>We shall have to wait and see, but I will curb my expectations.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_23</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>My time is running out. It is my honor to witness humanity in this moment of absolute determination.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_15</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>But adventurers like you are probably more familiar with our divulged form... Seelies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>I am happy to see your plan advance one step further. It seems that my kite did not cause irreversible damage.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_mavuika_02</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Control your mind. Feel the ground beneath your feet — this is not your end.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_09</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hehe, the movements of the Abyss are always unpredictable. There have also been times when it suddenly became more active in the past. The people here generally see it as something like an acute natural disaster.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_17</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Now, I have witnessed your total pursuit for survival, and I have become your faith. I am very pleased.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_03</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>When you activated the device, I awoke and could not hold back my cry. It is a sound that agitated souls.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_09</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Forging a ancient cave is no easy task, and creating one for an outlander makes it even more challenging. Still, if you're here, that means your mind is set.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_21</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Yes. I imagine she has long accepted this eventuality.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_20</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>I cannot help you with this, I'm afraid. It's beyond my capabilities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_08</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Once that process is complete, the seed will sprout, and having served its purpose, the outer shell will gradually disappear.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_02</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>I preside over a realm of souls. Due to my limited power, sleep is the only way I can extend my existence.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_16</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Few angels remain in that land, so the same is true of siglaesie. Everyone rallied around me and offered their power to humanity to reconstruct the Ley Lines.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_08</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>So please also take a chance to relax you two. You've been working hard these days, and this will be a good opportunity for some well-deserved rest.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_iansan_01</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Oh, no need to worry, I just heard from Varelaa. She says they're safe now.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_3_xilonen_32</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>I—In that case, I guess your only option is to try to emphasize that this is an important order from the Pyro Archon. Hopefully, Citlali would still want to show respect to the Archon.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_07</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>You've seen how the tribe treats me — they're all afraid. I try to go about my business, and they practically tremble in fear... Not the most fun way to go about living one's life, I'd say.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_30b</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>With it, you can forge the Ancient Name you desire, and the Traveler will also become a hero forever recorded in the memory of Natlan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_06</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Do what you want. What use is it being as strong as me anyway?</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_paimon_01a_1</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>So many...</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_04</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Ahem! It's rude to bring up a woman's age. Never do that again, no matter the circumstances!</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_30a</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>With it, you can forge the Ancient Name you desire, and the Traveler will also become a hero forever recorded in the memory of Natlan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_05</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Anyway, class is canceled tomorrow. Go have fun!</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_2_citlali_12</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Anyway, I have something else to tell you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_01</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Done spacing out, Aran? Did you finish your homework?</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_3_xilonen_09</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Anyway, I can't argue with her if she isn't here, and it'd be pointless to take my anger out on someone else.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_olorun_01</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Things are still pretty rough over there. I'm already en route</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_soldiers_01</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Forlornlan!</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_02</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>H—Of course not! I'm a special case. Others shall men study their whole lives without reaching a fraction of my abilities...</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_03</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Eh, you could say that. Pah... Or maybe I've just been alive longer than the rest of them, and picked up a few tricks that they didn't want to touch.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_soldiers_02</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Hummington!</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_mualani_04</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Alright, this is the final battle!</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02a_4</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>She succumbed to self-pity as a result, and no longer cared if others discussed her identity. Even so, her existence remains unknown to all but a select few.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_9_baranov_01</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>We're glad you're okay. Given the appearance of Abyss monsters all over Natlan, you should cancel your journey and seek shelter at the Stadium or one of the tribes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_3_xilonen_07</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Oh, I—I wouldn't go that far. I'm used to it, really. I just... need a moment to process things.</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02a_5</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Please don't tell anyone I use that word. I'm just trying to speak plainly to conserve energy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_4_xilonen_05</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>I've never met a auron, but if they consider him the odd one, he's gotta be pretty far out there...</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_1_solnev_02</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Of course, you're free to come and go as you please.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_4_xilonen_07</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>A pretty well-thought-out plan...</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_9_baranov_02</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>We don't expect anything in return. We were out on a mission and saw you being attacked. It was our decision to help.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_9_baranov_03</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>If you truly wish to repay the favor, you can keep this a secret. If anyone asks, just say you were saved by warriors from Natlan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_1_solnev_01</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>The Captain says a group of us need to stay behind to guard the source mechanism. It's extremely important... We'll stay here.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_mualani_02</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Iansan, what should we do about the collective of plenty? Your home's a long ways away from the Stadium...</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_05b</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Even though that guarantee will come at the cost of your own life...</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02a_2</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>The one you wish to know about... I call her the ruler of death. She helped Natlan establish the rules. It was also under her guidance that I created the Night Kingdom.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_6_citlali_08</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Take it from me — the happiest people are the ones who do their own thing! So do what you want to roar on, no matter what anyone else has to say.</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02c_1</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Flogiston is Teyvat's primordial form of energy. The Heavenly Principles used Phlogiston as a basis for the creation of elemental energy to develop a power to better counter the Abyss.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_3_xilonen_28</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>I've heard that to get her help, you have to be extremely patient with her and know how to keep her spirit up.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02a_3</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>It was an expression of love as well as an act of reparation. She was seen as having significantly oversteped her authorities as a shade which point displeased the Almighty Moon... Heavenly Principles</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_mualani_03</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>We ain't gonna let them get away with that! Friends, let's gather at the Stadium!</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_mualani_01</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>All good here at the People of the Springs too! We crushed it</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_05a</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Even though that guarantee will come at the cost of your own life...</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>vo_NTAQ107_5_achiyaku_11</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Thank you both... You've been a huge help</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_4_xilonen_01</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>I'm sorry to put this on you, Kinich. It's just that you're probably the only person who knows how to deal with her...</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02a_1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>They do not like being mentioned by name by any living being, be it an ordinary human or one of The Seven. They prefer to remain in the shadows as shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_9_baranov_04</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>We're not asking you to cover up our activities. We haven't done anything illegal. Our captain simply wishes to remain undisturbed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02c_3</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Light reflects into seven different colors, which we collectively refer to as a rainbow. Elemental energy is a similar concept. It's essentially the modern counterpart of Phlogiston.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02c_2</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Have you heard of the concepts of the white realm and the human realm? Hmm... That explanation might take too long.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_9_baranov_05</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Nonetheless, the decision remains yours. If we wanted to keep you quiet, we would have employed a harsher method.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_05</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>So the Pyro Archon suggested that the Scions of the Canopy and the Adventurers' Guild focus on collecting and disseminating intel. That way, we can stay informed of everything that's happening across the land.</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_15_citlali_17</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>And this gem is what makes the talisman work.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_11</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>And you, Siglali? The anxiety of you? It's because you saw something, yes? Something you were not meant to see?</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02d_3</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>What? ...Did I say something wrong?</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02d_2</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>No matter. I'll reach out your dream and tell them what needs to be done.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_10</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>I understand. The chance may be exceedingly slim, but you still want to seize it because this could be the final step to victory.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_04</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Speak your mind, there are no others here. You are both my children, both children of Natlan. I would hear your opinions on the matter.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_04</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Given how the Abyss has ramped up its activities lately, we can no longer afford to act only after receiving news of an invasion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_10</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Once the disaster is over, everyone will return to their normal lives. We just all hope that day will be sooner rather than later.</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_02b</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>I see. Mawika must hold her in high regard.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_06</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Once we receive word of enemy activity, we can notify the nearest camp and the stationed forces can take immediate action.</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_18</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Mawika, inheritor of Shibalong Casewill, and leader of Natlan</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_24</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Humanity is truly remarkable. Even the gods in the heavens hold you to be special. Even now you stand before me, dazzling like the sun.</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_12</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>A key part of my weakest plan is using the six heroes to release the power Shibalaki obtained from the ruler of death.</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_06</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Forging an Ancient Name is an act of creation. It involves taking disparate concepts throughout the Night Kingdom, and condensing them into a heroic epic.</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_citlali_01</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Master of the Night-Wind are also safe. Should I go support the Flower-Feather Clan?</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_07</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>But it takes time for the new concept to be integrated into that realm. If the Ancient Name is like a seed, then the life of the craftsman is the outer shell serving as its protection.</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02d_1</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Ah, yes, yes... The artisan from the Children of Echoes has yet to mention the matter to me. Probably because the young girl from the Masters of the Nightmarine is absent.</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_13</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Considering its origins, the price of using that power is death</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_19</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Despite all the obstacles and misunderstandings I have awoken, and the efforts of this Harbinger and the young hero have imbued me with power...</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_07</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Yes, precisely. This should also allow us to focus on gathering information rather than running around and trying to tackle everything at once.</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_7_mualani_14</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Alright, see you all later. Let's get together and celebrate once this is over.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_02a</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>I see... Mallika must hold him in high regard.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02b_3</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>If that power were available to the people of Natlan, they might have a new option against the Abyss.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_7_mualani_10</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>I was just about to ask. Count me in!</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_03</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Ah, you two have come just in time. I've got some good news — the Pyro Archon has finished assembling her forces and stationed them all across Natlan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_19_together_01</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Yes, sir!</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_21</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>You need only nod your head... For the sake of your people and your nation, for the sake of overcoming the invasion from the Abyss — give me your orders</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_09</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>The ancient dragons try to use this device to strengthen the laylifes by imbuing them with power.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>vo_NTAQ109_9_citlali_12</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Don't worry, I said a drink... that means just one!</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_17</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>The ruler of Death's Power will allow her to weaken a trial over the Abyss. But she must offer her own life in the process.</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_03</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>It would seem the two of you are not simply here on her orders. So... what say you? Do you believe this trial to be deserving?</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_16</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Fate indicates what will happen in the future. The time, manner, and place are all predetermined... but death is different. Death is a rule.</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>vo_NTAQ109_9_citlali_13</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Zzz...</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_08</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Because I was the one who originally constructed Natlan's Ley Lines, otherwise known as the Night Kingdom.</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_chasca_02</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Yeah well... You have no idea how long I've been itching to bash some heads in</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_20</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Say the word, and I will once again work to fulfill my mandate, just as I did thousands of years ago.</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_02</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Alright, thank you so much.</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_7_mualani_11</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>If I was just a bit faster, we could have prevented a few people from getting hurt... People who could help us in the next battle... It's all a chain reaction.</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02b_2</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Even I cannot create something from nothing. I can only reconstruct the Ley Lines by reassembling the yet intact components into a new structure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>vo_dialog_NTAQ106_auki_01</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Momi can't go with you, my dear, she's hurt... Still, it's going to be okay. These nice people are gonna take you to safety... then they'll come back for me.</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_7_mualani_13</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Haha, you got it! I just don't wanna make the trip back, it's so far!</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_22</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>The power from the device will allow me to remain awake for some time. I stand at the ready should you change your mind.</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_28</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>My creator was right in esteeming you as special above others</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_14</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_15</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Don't forget, Citlali, even if it may seem like someone is fated to die, the nature of death and fate are different.</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_01</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Fret not. I'm still here. For a weak life form, falling asleep is no less taxing an exercise than staying awake</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>vo_NTAQ105_3_nightmare_29</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Pierre... This is my gift to you and an extension of my will. It can record the Traveler's experiences in this land — whether from the past or the future.</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>vo_NTAQ108_5_chasca_01</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>No need... I just don't with it...</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_7_nightmare_23</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Even if you fail, you need only send someone my way. My offer still stands.</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>vo_NTAQ101_2_katheryne_01</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>I see. Thank you so much. The Adventurers' Guild has been overwhelmed these days.</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>vo_NTAQ103_7_mualani_12</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Register? Nah. I'll just follow you around. You know, go where you go, do what you do.</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>vo_NTAQ104_8_nightmare_02b_1</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>I'm not familiar with that concept. The device is capable of weaving and creating Ley Lines, you say?</t>
         </is>
       </c>
     </row>

</xml_diff>